<commit_message>
Fixed targeting and Stun-crash bug, cleaned up some debug messages
Fixed bug where spells would still hit dead enemies, and would crash the game if they were stunned. added Is_dead property to ICaster interface to accomplish this. Fixed after pause battle update to only update enemies death value if they are not already dead, removing uneccesary debug messages
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="66">
   <si>
     <t>name (root)</t>
   </si>
@@ -199,6 +199,24 @@
   </si>
   <si>
     <t>+crit rate, +casting time</t>
+  </si>
+  <si>
+    <t>kills self (debug)</t>
+  </si>
+  <si>
+    <t>mS</t>
+  </si>
+  <si>
+    <t>stun</t>
+  </si>
+  <si>
+    <t>deal stagger to all</t>
+  </si>
+  <si>
+    <t>LMR</t>
+  </si>
+  <si>
+    <t>death</t>
   </si>
 </sst>
 </file>
@@ -517,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +555,7 @@
     <col min="11" max="11" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -595,7 +613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -624,7 +642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -653,7 +671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -682,7 +700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -711,7 +729,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -740,7 +758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -769,7 +787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -798,231 +816,207 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>999</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K16" t="s">
-        <v>48</v>
-      </c>
-      <c r="L16" t="s">
-        <v>49</v>
-      </c>
-      <c r="M16" t="s">
-        <v>4</v>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="H17">
-        <v>1.2</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>1.25</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>1.25</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L18" t="s">
+        <v>49</v>
       </c>
       <c r="M18" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1">
         <v>0.75</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1037,27 +1031,27 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D20" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F20">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1066,10 +1060,10 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1083,28 +1077,28 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D21" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G21">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1119,11 +1113,93 @@
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>1.5</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22">
+        <v>1.5</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>-100</v>
+      </c>
+      <c r="H23">
+        <v>0.25</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Stat buff/debuffs, added elemental buff/debuffs
Added stat buff/debuffs, added roots that have inherent debuffs, added elemental buff/debuffs
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="84">
   <si>
     <t>name (root)</t>
   </si>
@@ -217,6 +217,60 @@
   </si>
   <si>
     <t>death</t>
+  </si>
+  <si>
+    <t>debilitate</t>
+  </si>
+  <si>
+    <t>buff</t>
+  </si>
+  <si>
+    <t>1 lvl of all non-elem debuffs</t>
+  </si>
+  <si>
+    <t>buff/debuffs</t>
+  </si>
+  <si>
+    <t>buff %</t>
+  </si>
+  <si>
+    <t>crush</t>
+  </si>
+  <si>
+    <t>applies def- debuff</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>prayer</t>
+  </si>
+  <si>
+    <t>1 lvl of all non-elem buffs</t>
+  </si>
+  <si>
+    <t>ADSHE</t>
+  </si>
+  <si>
+    <t>adshe</t>
+  </si>
+  <si>
+    <t>weakness</t>
+  </si>
+  <si>
+    <t>lowers target all elem resist</t>
+  </si>
+  <si>
+    <t>strength</t>
+  </si>
+  <si>
+    <t>increases all elem resist</t>
+  </si>
+  <si>
+    <t>UFIB</t>
+  </si>
+  <si>
+    <t>ufib</t>
   </si>
 </sst>
 </file>
@@ -535,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,11 +605,11 @@
     <col min="6" max="7" width="11.21875" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
     <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
     <col min="11" max="11" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -583,8 +637,14 @@
       <c r="I1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -612,8 +672,14 @@
       <c r="I2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -641,8 +707,14 @@
       <c r="I3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -670,8 +742,14 @@
       <c r="I4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -699,8 +777,14 @@
       <c r="I5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -728,25 +812,31 @@
       <c r="I6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <v>-1000</v>
+        <v>80</v>
       </c>
       <c r="G7">
         <v>10</v>
@@ -757,28 +847,34 @@
       <c r="I7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D8">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>-1000</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -786,19 +882,25 @@
       <c r="I8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>999</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -807,7 +909,7 @@
         <v>100</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -815,19 +917,25 @@
       <c r="I9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D10">
-        <v>999</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -836,27 +944,33 @@
         <v>100</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -865,86 +979,194 @@
         <v>100</v>
       </c>
       <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>100</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="G12">
+        <v>100</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
         <v>50</v>
       </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -954,252 +1176,325 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" t="s">
         <v>43</v>
-      </c>
-      <c r="G18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" t="s">
-        <v>46</v>
-      </c>
-      <c r="K18" t="s">
-        <v>48</v>
-      </c>
-      <c r="L18" t="s">
-        <v>49</v>
-      </c>
-      <c r="M18" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.75</v>
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>10</v>
-      </c>
-      <c r="H19">
-        <v>1.2</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1.25</v>
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>5</v>
-      </c>
-      <c r="F20">
-        <v>1.25</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>1.25</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.75</v>
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
       </c>
       <c r="E21">
         <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <v>1.5</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>10</v>
-      </c>
-      <c r="J22">
-        <v>1.5</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="M22" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>-100</v>
-      </c>
-      <c r="H23">
-        <v>0.25</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" t="s">
+        <v>46</v>
+      </c>
+      <c r="K23" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" t="s">
+        <v>49</v>
       </c>
       <c r="M23" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <v>1.2</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>1.25</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1.25</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>1.5</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="J27">
+        <v>1.5</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>-100</v>
+      </c>
+      <c r="H28">
+        <v>0.25</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added modFlag attribute to spells, allowing them to ignore certain types of mods
-no_mods makes the spell unmodifyable
-no_elements makes the spell unaffected by element mods
-no_styles makes the spell unaffected by style mods
-no_targeting makes the spell unaffect by styles that mod targeting.

FILES MODIFYED

spell.cs, spellDictionary.cs

TODO

-potentially make the flags bitflags so they can be used in combination? IDK if thats necessary
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
   <si>
     <t>name (root)</t>
   </si>
@@ -90,9 +90,6 @@
     <t>poke</t>
   </si>
   <si>
-    <t>high damage for debugging</t>
-  </si>
-  <si>
     <t>bolt</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>stun</t>
   </si>
   <si>
-    <t>deal stagger to all</t>
-  </si>
-  <si>
     <t>LMR</t>
   </si>
   <si>
@@ -307,6 +301,42 @@
   </si>
   <si>
     <t>lr</t>
+  </si>
+  <si>
+    <t>modFlag</t>
+  </si>
+  <si>
+    <t>high damage (debug)</t>
+  </si>
+  <si>
+    <t>deal stagger to all (debug)</t>
+  </si>
+  <si>
+    <t>quake</t>
+  </si>
+  <si>
+    <t>hits everyone!</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>no_targeting</t>
+  </si>
+  <si>
+    <t>no_mods</t>
+  </si>
+  <si>
+    <t>no_styles</t>
+  </si>
+  <si>
+    <t>nullify</t>
+  </si>
+  <si>
+    <t>can only deal null damage</t>
+  </si>
+  <si>
+    <t>no_elements</t>
   </si>
 </sst>
 </file>
@@ -342,9 +372,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,9 +674,10 @@
     <col min="9" max="9" width="10.77734375" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" customWidth="1"/>
     <col min="11" max="11" width="9.21875" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -665,22 +697,25 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -709,13 +744,13 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -744,13 +779,13 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -779,21 +814,21 @@
         <v>11</v>
       </c>
       <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>25</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -811,24 +846,24 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>40</v>
@@ -846,24 +881,24 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -884,21 +919,21 @@
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -919,13 +954,13 @@
         <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -933,7 +968,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="D9">
         <v>999</v>
@@ -954,21 +989,21 @@
         <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -989,21 +1024,21 @@
         <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11">
         <v>999</v>
@@ -1021,24 +1056,24 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D12">
         <v>25</v>
@@ -1056,24 +1091,24 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1091,100 +1126,106 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E14">
         <v>20</v>
       </c>
-      <c r="F14">
-        <v>100</v>
-      </c>
-      <c r="G14">
-        <v>10</v>
+      <c r="F14" s="2">
+        <v>85</v>
+      </c>
+      <c r="G14" s="2">
+        <v>25</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15">
+        <v>50</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2">
+        <v>90</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
         <v>11</v>
       </c>
-      <c r="J14" t="s">
-        <v>76</v>
-      </c>
-      <c r="K14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>50</v>
-      </c>
-      <c r="F15">
-        <v>100</v>
-      </c>
-      <c r="G15">
-        <v>10</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
-        <v>61</v>
-      </c>
       <c r="J15" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="K15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F16">
         <v>100</v>
@@ -1199,7 +1240,7 @@
         <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K16">
         <v>100</v>
@@ -1207,19 +1248,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F17">
         <v>100</v>
@@ -1231,10 +1272,10 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K17">
         <v>100</v>
@@ -1242,19 +1283,19 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>100</v>
@@ -1266,10 +1307,10 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="J18" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="K18">
         <v>100</v>
@@ -1277,34 +1318,34 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D19">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>100</v>
       </c>
       <c r="G19">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="J19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K19">
         <v>100</v>
@@ -1312,69 +1353,111 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
+      </c>
+      <c r="G20">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" t="s">
+        <v>90</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="L20" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" t="s">
-        <v>43</v>
+        <v>83</v>
+      </c>
+      <c r="D21">
+        <v>999</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <v>100</v>
+      </c>
+      <c r="G21">
+        <v>75</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1385,156 +1468,108 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26" t="s">
-        <v>45</v>
-      </c>
-      <c r="I26" t="s">
-        <v>47</v>
-      </c>
-      <c r="J26" t="s">
-        <v>46</v>
-      </c>
-      <c r="K26" t="s">
-        <v>48</v>
-      </c>
-      <c r="L26" t="s">
-        <v>49</v>
-      </c>
-      <c r="M26" t="s">
-        <v>4</v>
+        <v>34</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>10</v>
-      </c>
-      <c r="H27">
-        <v>1.2</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="M27" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28">
-        <v>10</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="E28">
-        <v>5</v>
-      </c>
-      <c r="F28">
-        <v>1.25</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>1.25</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" t="s">
+        <v>45</v>
+      </c>
+      <c r="K28" t="s">
+        <v>47</v>
+      </c>
+      <c r="L28" t="s">
+        <v>48</v>
       </c>
       <c r="M28" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D29" s="1">
         <v>0.75</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -1549,27 +1584,27 @@
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F30">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1578,10 +1613,10 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J30">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -1590,33 +1625,33 @@
         <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D31" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G31">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -1631,11 +1666,93 @@
         <v>1</v>
       </c>
       <c r="M31" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>1.5</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+      <c r="J32">
+        <v>1.5</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>-100</v>
+      </c>
+      <c r="H33">
+        <v>0.25</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added animationID and sfxID parameters to spells,element mods, style mods, and associated parsing code and excels
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="109">
   <si>
     <t>name (root)</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t>no_elements</t>
+  </si>
+  <si>
+    <t>anim ID</t>
+  </si>
+  <si>
+    <t>sfx ID</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -656,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,17 +676,19 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="9.21875" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="9" width="11.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.21875" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,34 +699,40 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>67</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>68</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -725,32 +742,38 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>85</v>
       </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -760,32 +783,38 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3">
         <v>20</v>
       </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
         <v>90</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>15</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -795,32 +824,38 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4">
         <v>30</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>15</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>75</v>
       </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>24</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -830,32 +865,38 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
+      <c r="D5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" t="s">
+        <v>108</v>
       </c>
       <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
         <v>75</v>
       </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
         <v>27</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>24</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -865,32 +906,38 @@
       <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6">
         <v>40</v>
       </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
         <v>95</v>
       </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
         <v>30</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>24</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -900,32 +947,38 @@
       <c r="C7" t="s">
         <v>70</v>
       </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" t="s">
+        <v>108</v>
       </c>
       <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
         <v>80</v>
       </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
         <v>11</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>71</v>
       </c>
-      <c r="K7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -935,32 +988,38 @@
       <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
       </c>
       <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>-1000</v>
       </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
         <v>11</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>24</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -970,32 +1029,38 @@
       <c r="C9" t="s">
         <v>95</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9">
         <v>999</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>100</v>
-      </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
         <v>11</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>24</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1005,32 +1070,38 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10">
         <v>2</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>100</v>
-      </c>
       <c r="G10">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
         <v>11</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>24</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -1040,32 +1111,38 @@
       <c r="C11" t="s">
         <v>59</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11">
         <v>999</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>100</v>
-      </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
         <v>60</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>24</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -1075,32 +1152,38 @@
       <c r="C12" t="s">
         <v>92</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12">
         <v>25</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>100</v>
-      </c>
       <c r="G12">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
         <v>93</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>24</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1110,32 +1193,38 @@
       <c r="C13" t="s">
         <v>96</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
+      <c r="D13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" t="s">
+        <v>108</v>
       </c>
       <c r="F13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
         <v>62</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>24</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -1145,35 +1234,41 @@
       <c r="C14" t="s">
         <v>98</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14">
         <v>50</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>20</v>
       </c>
-      <c r="F14" s="2">
+      <c r="H14" s="2">
         <v>85</v>
       </c>
-      <c r="G14" s="2">
+      <c r="I14" s="2">
         <v>25</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
         <v>99</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>24</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -1183,35 +1278,41 @@
       <c r="C15" t="s">
         <v>104</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15">
         <v>50</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>20</v>
       </c>
-      <c r="F15" s="2">
+      <c r="H15" s="2">
         <v>90</v>
       </c>
-      <c r="G15" s="2">
+      <c r="I15" s="2">
         <v>5</v>
       </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
         <v>11</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>24</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1221,32 +1322,38 @@
       <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
+      <c r="D16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
         <v>20</v>
       </c>
-      <c r="F16">
-        <v>100</v>
-      </c>
-      <c r="G16">
-        <v>10</v>
-      </c>
       <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
         <v>11</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>74</v>
       </c>
-      <c r="K16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -1256,32 +1363,38 @@
       <c r="C17" t="s">
         <v>73</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
+      <c r="D17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
         <v>50</v>
       </c>
-      <c r="F17">
-        <v>100</v>
-      </c>
-      <c r="G17">
-        <v>10</v>
-      </c>
       <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
         <v>60</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>75</v>
       </c>
-      <c r="K17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -1291,32 +1404,38 @@
       <c r="C18" t="s">
         <v>77</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
+      <c r="D18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" t="s">
+        <v>108</v>
       </c>
       <c r="F18">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
         <v>11</v>
       </c>
-      <c r="J18" t="s">
+      <c r="L18" t="s">
         <v>80</v>
       </c>
-      <c r="K18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1326,32 +1445,38 @@
       <c r="C19" t="s">
         <v>79</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" t="s">
+        <v>108</v>
       </c>
       <c r="F19">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
+        <v>100</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
         <v>60</v>
       </c>
-      <c r="J19" t="s">
+      <c r="L19" t="s">
         <v>81</v>
       </c>
-      <c r="K19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -1361,35 +1486,41 @@
       <c r="C20" t="s">
         <v>88</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
         <v>25</v>
       </c>
-      <c r="F20">
-        <v>100</v>
-      </c>
-      <c r="G20">
-        <v>10</v>
-      </c>
       <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
         <v>89</v>
       </c>
-      <c r="J20" t="s">
+      <c r="L20" t="s">
         <v>90</v>
       </c>
-      <c r="K20">
-        <v>100</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="M20">
+        <v>100</v>
+      </c>
+      <c r="N20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -1399,40 +1530,46 @@
       <c r="C21" t="s">
         <v>83</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21">
         <v>999</v>
       </c>
-      <c r="E21">
+      <c r="G21">
         <v>30</v>
       </c>
-      <c r="F21">
-        <v>100</v>
-      </c>
-      <c r="G21">
+      <c r="H21">
+        <v>100</v>
+      </c>
+      <c r="I21">
         <v>75</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
         <v>11</v>
       </c>
-      <c r="J21" t="s">
+      <c r="L21" t="s">
         <v>84</v>
       </c>
-      <c r="K21">
-        <v>100</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="M21">
+        <v>100</v>
+      </c>
+      <c r="N21" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1443,13 +1580,19 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" t="s">
         <v>49</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1459,14 +1602,20 @@
       <c r="C24" t="s">
         <v>32</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1476,14 +1625,20 @@
       <c r="C25" t="s">
         <v>33</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1493,19 +1648,25 @@
       <c r="C26" t="s">
         <v>34</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1516,37 +1677,43 @@
         <v>7</v>
       </c>
       <c r="D28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" t="s">
         <v>41</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>49</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
         <v>42</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>43</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>44</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>46</v>
       </c>
-      <c r="J28" t="s">
+      <c r="L28" t="s">
         <v>45</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>47</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>48</v>
       </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1556,38 +1723,44 @@
       <c r="C29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="1">
         <v>0.75</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
       <c r="G29">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>10</v>
+      </c>
+      <c r="J29">
         <v>1.2</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
         <v>1</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1597,38 +1770,44 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="1">
         <v>1.25</v>
       </c>
-      <c r="E30">
+      <c r="G30">
         <v>5</v>
       </c>
-      <c r="F30">
+      <c r="H30">
         <v>1.25</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
         <v>1.25</v>
       </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>1</v>
-      </c>
-      <c r="M30" t="s">
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1638,21 +1817,21 @@
       <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="1">
         <v>0.75</v>
       </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
       <c r="I31">
         <v>0</v>
       </c>
@@ -1665,11 +1844,17 @@
       <c r="L31">
         <v>1</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1679,38 +1864,44 @@
       <c r="C32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="1">
-        <v>1</v>
-      </c>
-      <c r="E32">
+      <c r="D32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32">
         <v>3</v>
       </c>
-      <c r="F32">
+      <c r="H32">
         <v>1.5</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
       <c r="I32">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>10</v>
+      </c>
+      <c r="L32">
         <v>1.5</v>
       </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>1</v>
-      </c>
-      <c r="M32" t="s">
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1720,38 +1911,44 @@
       <c r="C33" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="1">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
+      <c r="D33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
         <v>-100</v>
       </c>
-      <c r="H33">
+      <c r="J33">
         <v>0.25</v>
       </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
       <c r="K33">
         <v>0</v>
       </c>
       <c r="L33">
         <v>1</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added functionality for Repel popups, changed bolt to volt, changed elemental enums to be consisten with game
-Added functionality for repel popups to the game (sorry the system is so unituitive @stumpystool)
-Added spawnElementPopup method to BattleManager.cs to encapsulate element popup code
-Changed bolt to volt, icluding in the spellbook
-changes Elements.vsElement to be weak/resist/repel/block/drain instead of weak/resistant/reflect/abasorb

FILES MODIFIED:

uhh a lot idk
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -90,9 +90,6 @@
     <t>poke</t>
   </si>
   <si>
-    <t>bolt</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>adds ice element to spell</t>
   </si>
   <si>
-    <t>adds bolt element to spell</t>
-  </si>
-  <si>
     <t>+acc, -power</t>
   </si>
   <si>
@@ -346,6 +340,12 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>volt</t>
+  </si>
+  <si>
+    <t>adds volt element to spell</t>
   </si>
 </sst>
 </file>
@@ -668,7 +668,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,10 +699,10 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -714,22 +714,22 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
       </c>
       <c r="L1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -743,10 +743,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -767,7 +767,7 @@
         <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -784,10 +784,10 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F3">
         <v>20</v>
@@ -808,7 +808,7 @@
         <v>11</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -825,10 +825,10 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4">
         <v>30</v>
@@ -849,7 +849,7 @@
         <v>11</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -857,19 +857,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -887,10 +887,10 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -898,19 +898,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F6">
         <v>40</v>
@@ -928,10 +928,10 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -939,19 +939,19 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -972,7 +972,7 @@
         <v>11</v>
       </c>
       <c r="L7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M7">
         <v>100</v>
@@ -980,19 +980,19 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="L8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1027,13 +1027,13 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F9">
         <v>999</v>
@@ -1054,7 +1054,7 @@
         <v>11</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1062,19 +1062,19 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -1095,7 +1095,7 @@
         <v>11</v>
       </c>
       <c r="L10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1103,19 +1103,19 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F11">
         <v>999</v>
@@ -1133,10 +1133,10 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1144,19 +1144,19 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F12">
         <v>25</v>
@@ -1174,10 +1174,10 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1185,19 +1185,19 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1215,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1226,19 +1226,19 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F14">
         <v>50</v>
@@ -1256,33 +1256,33 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F15">
         <v>50</v>
@@ -1303,30 +1303,30 @@
         <v>11</v>
       </c>
       <c r="L15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1347,7 +1347,7 @@
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M16">
         <v>100</v>
@@ -1355,19 +1355,19 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1385,10 +1385,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M17">
         <v>100</v>
@@ -1396,19 +1396,19 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1429,7 +1429,7 @@
         <v>11</v>
       </c>
       <c r="L18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M18">
         <v>100</v>
@@ -1437,40 +1437,40 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" t="s">
         <v>79</v>
-      </c>
-      <c r="D19" t="s">
-        <v>108</v>
-      </c>
-      <c r="E19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>100</v>
-      </c>
-      <c r="I19">
-        <v>10</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19" t="s">
-        <v>60</v>
-      </c>
-      <c r="L19" t="s">
-        <v>81</v>
       </c>
       <c r="M19">
         <v>100</v>
@@ -1478,19 +1478,19 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
         <v>86</v>
       </c>
-      <c r="B20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" t="s">
-        <v>88</v>
-      </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1508,33 +1508,33 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M20">
         <v>100</v>
       </c>
       <c r="N20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F21">
         <v>999</v>
@@ -1555,13 +1555,13 @@
         <v>11</v>
       </c>
       <c r="L21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M21">
         <v>100</v>
       </c>
       <c r="N21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -1580,16 +1580,16 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -1600,13 +1600,13 @@
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1623,13 +1623,13 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1640,19 +1640,19 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1671,43 +1671,43 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" t="s">
         <v>41</v>
       </c>
-      <c r="G28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>42</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
+        <v>44</v>
+      </c>
+      <c r="L28" t="s">
         <v>43</v>
       </c>
-      <c r="J28" t="s">
-        <v>44</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
+        <v>45</v>
+      </c>
+      <c r="N28" t="s">
         <v>46</v>
-      </c>
-      <c r="L28" t="s">
-        <v>45</v>
-      </c>
-      <c r="M28" t="s">
-        <v>47</v>
-      </c>
-      <c r="N28" t="s">
-        <v>48</v>
       </c>
       <c r="O28" t="s">
         <v>4</v>
@@ -1721,13 +1721,13 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F29" s="1">
         <v>0.75</v>
@@ -1757,24 +1757,24 @@
         <v>1</v>
       </c>
       <c r="O29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B30">
         <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F30" s="1">
         <v>1.25</v>
@@ -1804,24 +1804,24 @@
         <v>1</v>
       </c>
       <c r="O30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F31" s="1">
         <v>0.75</v>
@@ -1851,24 +1851,24 @@
         <v>1</v>
       </c>
       <c r="O31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -1898,24 +1898,24 @@
         <v>1</v>
       </c>
       <c r="O32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
@@ -1945,7 +1945,7 @@
         <v>1</v>
       </c>
       <c r="O33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Moved Player UI Up more, and others
- UI is higher now (w/ a frame change)
- lowered Lance cooldown
- player battle name field now updates properly
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +808,7 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H3">
         <v>95</v>

</xml_diff>

<commit_message>
Added animation and sfx system, added more animations
-All animations added during this branch: stab anim, volt anim, slash anim (10 frames version), explosion anim (used as crush, is 12 frames)
-Effects processing handled in SpellEffects.cs
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spellDictionary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="124">
   <si>
     <t>name (root)</t>
   </si>
@@ -318,9 +318,6 @@
     <t>sfx ID</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>volt</t>
   </si>
   <si>
@@ -361,12 +358,45 @@
   </si>
   <si>
     <t>Override ATK type to Volt</t>
+  </si>
+  <si>
+    <t>anim_spell_slash</t>
+  </si>
+  <si>
+    <t>animation ID</t>
+  </si>
+  <si>
+    <t>sfx_slash</t>
+  </si>
+  <si>
+    <t>sfx_stab</t>
+  </si>
+  <si>
+    <t>sfx_crush</t>
+  </si>
+  <si>
+    <t>anim_spell_volt</t>
+  </si>
+  <si>
+    <t>sfx_fire_hit</t>
+  </si>
+  <si>
+    <t>sfx_ice_hit</t>
+  </si>
+  <si>
+    <t>sfx_volt_hit</t>
+  </si>
+  <si>
+    <t>anim_spell_stab</t>
+  </si>
+  <si>
+    <t>anim_spell_crush</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -679,31 +709,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +744,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="E1" t="s">
         <v>98</v>
@@ -747,7 +777,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -755,13 +785,13 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -788,21 +818,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="F3">
         <v>20</v>
@@ -829,21 +859,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="F4">
         <v>30</v>
@@ -870,21 +900,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F5">
         <v>-30</v>
@@ -911,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -922,10 +952,10 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -952,7 +982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -963,10 +993,10 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F7">
         <v>40</v>
@@ -993,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -1004,10 +1034,10 @@
         <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -1034,7 +1064,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1045,10 +1075,10 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1075,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1086,10 +1116,10 @@
         <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F10">
         <v>999</v>
@@ -1116,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1127,10 +1157,10 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -1157,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1168,10 +1198,10 @@
         <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F12">
         <v>999</v>
@@ -1198,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -1209,10 +1239,10 @@
         <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F13">
         <v>25</v>
@@ -1239,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1250,10 +1280,10 @@
         <v>87</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1280,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -1291,10 +1321,10 @@
         <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F15">
         <v>50</v>
@@ -1324,7 +1354,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1335,10 +1365,10 @@
         <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F16">
         <v>50</v>
@@ -1368,7 +1398,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1379,10 +1409,10 @@
         <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1409,7 +1439,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1420,10 +1450,10 @@
         <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1450,7 +1480,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1461,10 +1491,10 @@
         <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1491,7 +1521,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1502,10 +1532,10 @@
         <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1532,7 +1562,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -1543,10 +1573,10 @@
         <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1576,7 +1606,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -1587,10 +1617,10 @@
         <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F22">
         <v>999</v>
@@ -1620,12 +1650,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1648,21 +1678,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1671,44 +1701,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
       </c>
       <c r="C26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" t="s">
         <v>112</v>
       </c>
-      <c r="D26" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" t="s">
-        <v>99</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>107</v>
-      </c>
-      <c r="B27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" t="s">
-        <v>113</v>
-      </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="E27" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1717,12 +1747,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1769,7 +1799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1779,11 +1809,11 @@
       <c r="C30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>99</v>
+      <c r="D30" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" t="s">
+        <v>115</v>
       </c>
       <c r="F30" s="1">
         <v>0.75</v>
@@ -1816,7 +1846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1826,11 +1856,11 @@
       <c r="C31" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>99</v>
+      <c r="D31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" t="s">
+        <v>115</v>
       </c>
       <c r="F31" s="1">
         <v>1.25</v>
@@ -1863,7 +1893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1873,11 +1903,11 @@
       <c r="C32" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>99</v>
+      <c r="D32" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" t="s">
+        <v>115</v>
       </c>
       <c r="F32" s="1">
         <v>0.75</v>
@@ -1910,7 +1940,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1920,11 +1950,11 @@
       <c r="C33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>99</v>
+      <c r="D33" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" t="s">
+        <v>115</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
@@ -1957,7 +1987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1967,11 +1997,11 @@
       <c r="C34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>99</v>
+      <c r="D34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" t="s">
+        <v>115</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
@@ -2004,7 +2034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added fire, updated smash animation
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="125">
   <si>
     <t>name (root)</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>anim_spell_crush</t>
+  </si>
+  <si>
+    <t>anim_spell_fire</t>
   </si>
 </sst>
 </file>
@@ -713,7 +716,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1689,7 +1692,7 @@
         <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E25" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Added ice, heal, empower animations to the game
NOTES:
Ice is bigger than our standard format, but works fine at 64 PPU
Heal is currently too long, coming in at a whopping 30 frames.
Empower might be also too long for a spell anim (16 frames) but I have may have misunderstood its purpose (it might be the enemy pre-cast animation)
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496E5452-4ABA-43F7-9E26-86CFB7017372}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="128">
   <si>
     <t>name (root)</t>
   </si>
@@ -394,6 +395,15 @@
   </si>
   <si>
     <t>anim_spell_fire</t>
+  </si>
+  <si>
+    <t>anim_spell_ice</t>
+  </si>
+  <si>
+    <t>anim_spell_empower</t>
+  </si>
+  <si>
+    <t>anim_spell_heal</t>
   </si>
 </sst>
 </file>
@@ -715,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,7 +734,7 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
@@ -914,7 +924,7 @@
         <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
         <v>115</v>
@@ -1715,7 +1725,7 @@
         <v>111</v>
       </c>
       <c r="D26" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E26" t="s">
         <v>120</v>
@@ -1813,7 +1823,7 @@
         <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E30" t="s">
         <v>115</v>
@@ -1860,7 +1870,7 @@
         <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E31" t="s">
         <v>115</v>
@@ -1907,7 +1917,7 @@
         <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E32" t="s">
         <v>115</v>
@@ -1954,7 +1964,7 @@
         <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E33" t="s">
         <v>115</v>
@@ -2001,7 +2011,7 @@
         <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E34" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
Added Stinger Spell to Test Interrupt Bug
- use stinger on the last enemy in the Changeling / Tanuki / Changeling wave
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/spellDictionary.xlsx
+++ b/Typocrypha/Assets/excel/spellDictionary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF1FBC85-D564-47A3-8C53-64B0CADF02C5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ACAEC5-F0E0-44A5-8A00-CA12ADA9580A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="134">
   <si>
     <t>name (root)</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>Does Nothing</t>
+  </si>
+  <si>
+    <t>stinger</t>
+  </si>
+  <si>
+    <t>High Dmg Critical Hit</t>
   </si>
 </sst>
 </file>
@@ -735,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,57 +1384,54 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="D16" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F16">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G16">
-        <v>20</v>
-      </c>
-      <c r="H16" s="2">
-        <v>85</v>
-      </c>
-      <c r="I16" s="2">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>9999</v>
+      </c>
+      <c r="I16">
+        <v>9999</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="L16" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D17" t="s">
         <v>112</v>
@@ -1443,16 +1446,16 @@
         <v>20</v>
       </c>
       <c r="H17" s="2">
+        <v>85</v>
+      </c>
+      <c r="I17" s="2">
+        <v>25</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
         <v>90</v>
-      </c>
-      <c r="I17" s="2">
-        <v>5</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0</v>
-      </c>
-      <c r="K17" t="s">
-        <v>10</v>
       </c>
       <c r="L17" t="s">
         <v>18</v>
@@ -1461,18 +1464,18 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
         <v>112</v>
@@ -1481,39 +1484,42 @@
         <v>114</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="G18">
         <v>20</v>
       </c>
-      <c r="H18">
-        <v>100</v>
-      </c>
-      <c r="I18">
-        <v>10</v>
-      </c>
-      <c r="J18">
+      <c r="H18" s="2">
+        <v>90</v>
+      </c>
+      <c r="I18" s="2">
+        <v>5</v>
+      </c>
+      <c r="J18" s="2">
         <v>0</v>
       </c>
       <c r="K18" t="s">
         <v>10</v>
       </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="M18">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
         <v>112</v>
@@ -1525,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H19">
         <v>100</v>
@@ -1537,10 +1543,10 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M19">
         <v>100</v>
@@ -1548,13 +1554,13 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
         <v>112</v>
@@ -1566,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="H20">
         <v>100</v>
@@ -1578,10 +1584,10 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="L20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="M20">
         <v>100</v>
@@ -1589,13 +1595,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>112</v>
@@ -1619,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="L21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M21">
         <v>100</v>
@@ -1630,13 +1636,13 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>112</v>
@@ -1648,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <v>100</v>
@@ -1660,27 +1666,24 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="L22" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M22">
         <v>100</v>
-      </c>
-      <c r="N22" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D23" t="s">
         <v>112</v>
@@ -1689,99 +1692,120 @@
         <v>114</v>
       </c>
       <c r="F23">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H23">
         <v>100</v>
       </c>
       <c r="I23">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="L23" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M23">
         <v>100</v>
       </c>
       <c r="N23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24">
+        <v>999</v>
+      </c>
+      <c r="G24">
+        <v>30</v>
+      </c>
+      <c r="H24">
+        <v>100</v>
+      </c>
+      <c r="I24">
+        <v>75</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" t="s">
+        <v>75</v>
+      </c>
+      <c r="M24">
+        <v>100</v>
+      </c>
+      <c r="N24" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="E26" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="F26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1792,19 +1816,19 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1815,112 +1839,88 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>105</v>
+      </c>
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" t="s">
-        <v>33</v>
-      </c>
-      <c r="I30" t="s">
-        <v>34</v>
-      </c>
-      <c r="J30" t="s">
-        <v>35</v>
-      </c>
-      <c r="K30" t="s">
-        <v>37</v>
-      </c>
-      <c r="L30" t="s">
-        <v>36</v>
-      </c>
-      <c r="M30" t="s">
-        <v>38</v>
-      </c>
-      <c r="N30" t="s">
-        <v>39</v>
-      </c>
-      <c r="O30" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="E31" t="s">
-        <v>114</v>
-      </c>
-      <c r="F31" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <v>10</v>
-      </c>
-      <c r="J31">
-        <v>1.2</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>1</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="F31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" t="s">
+        <v>35</v>
+      </c>
+      <c r="K31" t="s">
+        <v>37</v>
+      </c>
+      <c r="L31" t="s">
+        <v>36</v>
+      </c>
+      <c r="M31" t="s">
+        <v>38</v>
+      </c>
+      <c r="N31" t="s">
+        <v>39</v>
       </c>
       <c r="O31" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="B32">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
         <v>125</v>
@@ -1929,25 +1929,25 @@
         <v>114</v>
       </c>
       <c r="F32" s="1">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="G32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
       <c r="L32">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -1961,13 +1961,13 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D33" t="s">
         <v>125</v>
@@ -1976,13 +1976,13 @@
         <v>114</v>
       </c>
       <c r="F33" s="1">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H33">
-        <v>1.1499999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -1994,7 +1994,7 @@
         <v>0</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -2003,18 +2003,18 @@
         <v>1</v>
       </c>
       <c r="O33" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
         <v>125</v>
@@ -2023,13 +2023,13 @@
         <v>114</v>
       </c>
       <c r="F34" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H34">
-        <v>1.5</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2038,10 +2038,10 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L34">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="M34">
         <v>0</v>
@@ -2050,18 +2050,18 @@
         <v>1</v>
       </c>
       <c r="O34" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
         <v>125</v>
@@ -2073,22 +2073,22 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I35">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -2102,6 +2102,53 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>-100</v>
+      </c>
+      <c r="J36">
+        <v>0.25</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>